<commit_message>
Added cumulative spend chart
</commit_message>
<xml_diff>
--- a/gui/raw_data.xlsx
+++ b/gui/raw_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kimi/Documents/GitHub/Python-Spending-tracker-project/gui/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42968423-3E92-0849-BB76-123AAB85B18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A32118-2337-AE49-9A56-53592766E5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17100" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{2A48221C-6C62-284F-B749-38FE58A11E78}"/>
   </bookViews>
@@ -1024,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453D5E31-C30D-C347-88B4-AA0F28CAA586}">
   <dimension ref="A1:F397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" workbookViewId="0">
-      <selection activeCell="E409" sqref="E409"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>